<commit_message>
Opravena chyba: vrácena je první nalezená otázka na požadované úrovni.
</commit_message>
<xml_diff>
--- a/Melichar_Milionar/otazky.xlsx
+++ b/Melichar_Milionar/otazky.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ondřej Melichar\VAH\WPF\Melichar_Milionar\Melichar_Milionar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ondřej Melichar\Moje data\škola\3. ročník\VAH\WPF\Melichar_Milionar\Melichar_Milionar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A5B875-824B-466B-B4CC-1467C0A85845}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Jaké z vybraných slov neexistuje?</t>
   </si>
@@ -116,12 +112,27 @@
   </si>
   <si>
     <t>Jaký je správný zápis čísla 3 v binární soustavě?</t>
+  </si>
+  <si>
+    <t>Pro kola je typycký/á/é:</t>
+  </si>
+  <si>
+    <t>bradka</t>
+  </si>
+  <si>
+    <t>hříva</t>
+  </si>
+  <si>
+    <t>ploutev</t>
+  </si>
+  <si>
+    <t>tesáky</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -467,11 +478,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,6 +654,26 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Funkční a nadesignovaný výpis statistik. Chybí pouze tlačítko pro návrat do hlavního menu.
</commit_message>
<xml_diff>
--- a/Melichar_Milionar/otazky.xlsx
+++ b/Melichar_Milionar/otazky.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ondřej Melichar\Moje data\škola\3. ročník\VAH\WPF\Melichar_Milionar\Melichar_Milionar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A043AD5-9FB5-452C-811E-F44C39F99DCD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DEFAFA-B6DB-4CAD-AA2D-19A44C6A0099}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>Jaký je správný zápis čísla 3 v binární soustavě?</t>
   </si>
   <si>
-    <t>Pro kola je typycký/á/é:</t>
-  </si>
-  <si>
     <t>bradka</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>5.</t>
+  </si>
+  <si>
+    <t>Pro kozla je typycký/á/é:</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,39 +674,39 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>1996</v>
-      </c>
-      <c r="D4">
-        <v>1998</v>
-      </c>
-      <c r="E4">
-        <v>2004</v>
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -714,39 +714,39 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>1996</v>
+      </c>
+      <c r="D5">
+        <v>1998</v>
+      </c>
+      <c r="E5">
+        <v>2004</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -754,79 +754,79 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>111</v>
-      </c>
-      <c r="D8">
-        <v>101</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>111</v>
+      </c>
+      <c r="D9">
+        <v>101</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
       </c>
       <c r="F10">
         <v>6</v>
@@ -834,19 +834,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -854,19 +854,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
       </c>
       <c r="F12">
         <v>8</v>
@@ -874,19 +874,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>57</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
       </c>
       <c r="F13">
         <v>9</v>
@@ -894,19 +894,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
         <v>59</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>62</v>
-      </c>
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>63</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -914,19 +914,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>66</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>67</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
       </c>
       <c r="F15">
         <v>11</v>
@@ -934,19 +934,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>71</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>72</v>
-      </c>
-      <c r="E16" t="s">
-        <v>73</v>
       </c>
       <c r="F16">
         <v>12</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -974,19 +974,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>76</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>77</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>78</v>
-      </c>
-      <c r="E18" t="s">
-        <v>79</v>
       </c>
       <c r="F18">
         <v>14</v>
@@ -994,25 +994,28 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" t="s">
-        <v>48</v>
       </c>
       <c r="F19">
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:F19">
+    <sortCondition ref="F1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>